<commit_message>
SAE-303 - Update dataset
</commit_message>
<xml_diff>
--- a/integration-web-s3/sae-303/datasets/developpement/geo-top-5-sports-avec-plus-licencies-par-region-2023-france.xlsx
+++ b/integration-web-s3/sae-303/datasets/developpement/geo-top-5-sports-avec-plus-licencies-par-region-2023-france.xlsx
@@ -24,13 +24,14 @@
     <sheet name="94 - Corse" sheetId="15" r:id="rId15"/>
     <sheet name="COM - COM" sheetId="16" r:id="rId16"/>
     <sheet name="980 - Monaco" sheetId="17" r:id="rId17"/>
+    <sheet name="Toutes" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="60">
   <si>
     <t>région</t>
   </si>
@@ -204,6 +205,12 @@
   </si>
   <si>
     <t>980</t>
+  </si>
+  <si>
+    <t>Toutes</t>
+  </si>
+  <si>
+    <t>Tous</t>
   </si>
 </sst>
 </file>
@@ -2638,6 +2645,117 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2">
+        <v>2215848</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3">
+        <v>1106989</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4">
+        <v>675186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5">
+        <v>594408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6">
+        <v>531864</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>

</xml_diff>